<commit_message>
Chose a few tests
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\cravethedave\masters\minicpbp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A53394-C38A-4DB8-85A5-2317F7B652A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E641E42-3BDF-4134-A803-41DA98CE5F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="My pc" sheetId="1" r:id="rId1"/>
+    <sheet name="ComputeCanada" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>MinWt</t>
   </si>
@@ -383,14 +384,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="11.28515625" style="1" customWidth="1"/>
-    <col min="7" max="10" width="11.42578125" style="1" customWidth="1"/>
+    <col min="1" max="6" width="11.42578125" style="1" customWidth="1"/>
+    <col min="7" max="10" width="12.140625" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -591,8 +592,12 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="I7" s="3">
+        <v>170597</v>
+      </c>
+      <c r="J7" s="3">
+        <v>46204</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G8" s="3"/>
@@ -721,4 +726,201 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19EE866B-4C8C-4265-8D9B-CBA7AC19948D}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="10" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2996</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3000</v>
+      </c>
+      <c r="C3" s="1">
+        <v>35</v>
+      </c>
+      <c r="D3" s="1">
+        <v>65</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2996</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3000</v>
+      </c>
+      <c r="C4" s="1">
+        <v>35</v>
+      </c>
+      <c r="D4" s="1">
+        <v>65</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2996</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3000</v>
+      </c>
+      <c r="C5" s="1">
+        <v>35</v>
+      </c>
+      <c r="D5" s="1">
+        <v>65</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2500</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3000</v>
+      </c>
+      <c r="C6" s="1">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
+        <v>90</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2975</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3050</v>
+      </c>
+      <c r="C7" s="1">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1">
+        <v>90</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>